<commit_message>
DONE - Adicionando livros inseridos no backend à lista de procura TODO - Atualizar o readme para os procedimentos com o backend
</commit_message>
<xml_diff>
--- a/grade-horas.xlsx
+++ b/grade-horas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vitor\Documents\apps\nodeapps\foton-exame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4171BB0E-8CCA-4755-A34E-CF5262DFF503}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514B6A80-8C2A-4107-84BA-59F8729BA056}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9072" xr2:uid="{5EEFD653-7919-4C54-8B13-78F4DECC86AD}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Dia</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>19h</t>
+  </si>
+  <si>
+    <t>24H</t>
   </si>
 </sst>
 </file>
@@ -472,7 +475,9 @@
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F12" s="1"/>

</xml_diff>

<commit_message>
DONE - Posicionamento de alguns itens decorativos do sistema DONE - Atualização do readme e da grade de horários
</commit_message>
<xml_diff>
--- a/grade-horas.xlsx
+++ b/grade-horas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vitor\Documents\apps\nodeapps\foton-exame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514B6A80-8C2A-4107-84BA-59F8729BA056}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D804330-1724-4170-9A36-84102259902C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9072" xr2:uid="{5EEFD653-7919-4C54-8B13-78F4DECC86AD}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Dia</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>24H</t>
+  </si>
+  <si>
+    <t>Quarta</t>
+  </si>
+  <si>
+    <t>17h40</t>
   </si>
 </sst>
 </file>
@@ -427,7 +433,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,6 +485,17 @@
         <v>10</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F12" s="1"/>
     </row>

</xml_diff>